<commit_message>
Manas's Commit 5th Mar 10:27 a.m.
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311DBB2F-B4C6-4075-A1B6-33F52D7AE27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7962E71E-B232-4E61-AF1E-746634BBB2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="258">
   <si>
     <t>Test Name</t>
   </si>
@@ -758,6 +758,69 @@
   </si>
   <si>
     <t>test_Prop2Agrmnt_Turbo</t>
+  </si>
+  <si>
+    <t>test_TC_011_ManualAdjustments</t>
+  </si>
+  <si>
+    <t>test_ManualAdjustment_Classic</t>
+  </si>
+  <si>
+    <t>test_ManualAdjustment_Turbo</t>
+  </si>
+  <si>
+    <t>test_ManualAdjustment_Split</t>
+  </si>
+  <si>
+    <t>test_TC_012_Approval</t>
+  </si>
+  <si>
+    <t>test_Approval_Classic</t>
+  </si>
+  <si>
+    <t>test_Approval_Turbo</t>
+  </si>
+  <si>
+    <t>Not Supported - CPQ-40251</t>
+  </si>
+  <si>
+    <t>test_Approval_Split</t>
+  </si>
+  <si>
+    <t>test_TC_013_CR_Inclusion</t>
+  </si>
+  <si>
+    <t>test_CR_Inclusion_Classic</t>
+  </si>
+  <si>
+    <t>test_CR_Inclusion_Split</t>
+  </si>
+  <si>
+    <t>test_CR_Inclusion_Turbo</t>
+  </si>
+  <si>
+    <t>test_DealGuidance_Classic</t>
+  </si>
+  <si>
+    <t>test_TC_014_TestDealGuidance</t>
+  </si>
+  <si>
+    <t>test_DealGuidance_Split</t>
+  </si>
+  <si>
+    <t>test_DealGuidance_Turbo</t>
+  </si>
+  <si>
+    <t>test_TC_015_TestPriceMatrix</t>
+  </si>
+  <si>
+    <t>test_PriceMatrix_Classic</t>
+  </si>
+  <si>
+    <t>test_PriceMatrix_Split</t>
+  </si>
+  <si>
+    <t>test_PriceMatrix_Turbo</t>
   </si>
 </sst>
 </file>
@@ -861,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -886,11 +949,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1174,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE8C29B-2DBF-44E9-93DE-0354258C5C49}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1274,10 +1336,10 @@
       <c r="C7" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="9" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1515,8 +1577,158 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="C34" s="15"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>11</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>12</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>13</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>14</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>15</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Manas's Commit 5th Mar 12.29 p.m.
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7962E71E-B232-4E61-AF1E-746634BBB2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAB51FB-D7D8-48A3-B896-45C17887092C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs Status" sheetId="18" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="266">
   <si>
     <t>Test Name</t>
   </si>
@@ -565,9 +565,6 @@
     <t>MN - 2020 Proposal TC_015</t>
   </si>
   <si>
-    <t>MN - 2020 Standalone PP (PriceMatrix)</t>
-  </si>
-  <si>
     <t>test_PriceWaterfall</t>
   </si>
   <si>
@@ -821,6 +818,33 @@
   </si>
   <si>
     <t>test_PriceMatrix_Turbo</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>rgb(25,146,229)</t>
+  </si>
+  <si>
+    <t>USD 100.00000</t>
+  </si>
+  <si>
+    <t>PM-0000000456</t>
+  </si>
+  <si>
+    <t>rgb(255,94,25)</t>
+  </si>
+  <si>
+    <t>(USD 5.00000)</t>
+  </si>
+  <si>
+    <t>Base Price</t>
+  </si>
+  <si>
+    <t>USD 95.00000</t>
+  </si>
+  <si>
+    <t>MN - 2020 Standalone (PriceMatrix)</t>
   </si>
 </sst>
 </file>
@@ -924,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -955,6 +979,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE8C29B-2DBF-44E9-93DE-0354258C5C49}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -1255,22 +1280,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>192</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,22 +1303,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1315,7 +1340,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1323,32 +1348,32 @@
         <v>3</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1356,29 +1381,29 @@
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>208</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,29 +1411,29 @@
         <v>5</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>212</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,29 +1441,29 @@
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>216</v>
-      </c>
       <c r="E15" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,29 +1471,29 @@
         <v>7</v>
       </c>
       <c r="B18" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>220</v>
-      </c>
       <c r="E18" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,29 +1501,29 @@
         <v>8</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>224</v>
-      </c>
       <c r="E21" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1506,29 +1531,29 @@
         <v>9</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>228</v>
-      </c>
       <c r="E24" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,45 +1561,45 @@
         <v>10</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>232</v>
-      </c>
       <c r="E27" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,29 +1607,29 @@
         <v>11</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>238</v>
-      </c>
       <c r="E32" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C33" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,32 +1637,32 @@
         <v>12</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>242</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C36" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,29 +1670,29 @@
         <v>13</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>247</v>
-      </c>
       <c r="E38" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,29 +1700,29 @@
         <v>14</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,29 +1730,29 @@
         <v>15</v>
       </c>
       <c r="B44" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>255</v>
-      </c>
       <c r="E44" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C46" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1978,7 +2003,7 @@
         <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +2011,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,7 +2019,7 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2033,7 +2058,7 @@
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,7 +2072,7 @@
         <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,7 +2086,7 @@
         <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2075,7 +2100,7 @@
         <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2089,7 +2114,7 @@
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,7 +2128,7 @@
         <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,7 +2142,7 @@
         <v>104</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2156,7 @@
         <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2145,7 +2170,7 @@
         <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,7 +2184,7 @@
         <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,7 +2198,7 @@
         <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2187,7 +2212,7 @@
         <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2650,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,7 +2735,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2720,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,11 +2760,13 @@
     <col min="5" max="5" width="16" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="8" max="8" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2761,16 +2788,25 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2782,7 +2818,27 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>265</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manas's Commit 5th Mar 02:24 p.m.
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAB51FB-D7D8-48A3-B896-45C17887092C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E1A2B5-67AD-4C4A-90B3-DFA4ED80A70A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs Status" sheetId="18" r:id="rId1"/>
@@ -1263,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE8C29B-2DBF-44E9-93DE-0354258C5C49}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -1658,7 +1658,7 @@
       <c r="C37" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="14" t="s">
         <v>203</v>
       </c>
       <c r="F37" s="9" t="s">
@@ -2490,7 +2490,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,7 +2675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
8th Mar 10:53 a.m. Manas's commit
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AF2D48-FBC5-47A7-913C-C4F5E5EFCA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A675C556-CA1E-485F-AB81-B5D64970F308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="275">
   <si>
     <t>Test Name</t>
   </si>
@@ -867,6 +867,12 @@
   </si>
   <si>
     <t>O2O Action Option Prd</t>
+  </si>
+  <si>
+    <t>MN - 2020 Option 1 is excluded on the addition of MN - 2020 BUNDLE (ConstRule)</t>
+  </si>
+  <si>
+    <t>MN - 2020 Option 3 is excluded on the addition of MN - 2020 Option 2</t>
   </si>
 </sst>
 </file>
@@ -2870,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D72C41-A294-471A-A10F-81DBDBC72609}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,6 +2959,14 @@
       </c>
       <c r="J2" s="5" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
9th Mar 04:47 p.m. Manas's commit
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A675C556-CA1E-485F-AB81-B5D64970F308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF3A8A2-6D9A-4D4D-BA58-2BA1ABF633D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs Status" sheetId="18" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="TC_015" sheetId="16" r:id="rId17"/>
     <sheet name="TC_016" sheetId="17" r:id="rId18"/>
     <sheet name="TC_017" sheetId="19" r:id="rId19"/>
+    <sheet name="TC_018" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="286">
   <si>
     <t>Test Name</t>
   </si>
@@ -873,6 +874,39 @@
   </si>
   <si>
     <t>MN - 2020 Option 3 is excluded on the addition of MN - 2020 Option 2</t>
+  </si>
+  <si>
+    <t>test_Allow Manaul Adj False</t>
+  </si>
+  <si>
+    <t>MN - 2020 Proposal TC_018</t>
+  </si>
+  <si>
+    <t>MN - 2020 BUNDLE 1</t>
+  </si>
+  <si>
+    <t>Option Prd</t>
+  </si>
+  <si>
+    <t>MN - 2020 Option (Alw Adj False)</t>
+  </si>
+  <si>
+    <t>MN - 2020 BUNDLE 2</t>
+  </si>
+  <si>
+    <t>MN - 2020 Option (Alw Adj False) (Inside SubBundle)</t>
+  </si>
+  <si>
+    <t>test_TC_017_CR_Exclusion</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Disable_Selection_Classic</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Disable_Selection_Split</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Disable_Selection_TP</t>
   </si>
 </sst>
 </file>
@@ -1289,17 +1323,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE8C29B-2DBF-44E9-93DE-0354258C5C49}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="9" customWidth="1"/>
     <col min="2" max="2" width="69" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="9" customWidth="1"/>
     <col min="6" max="6" width="27.140625" style="9" customWidth="1"/>
@@ -1780,6 +1814,36 @@
         <v>256</v>
       </c>
       <c r="E46" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>17</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>195</v>
       </c>
     </row>
@@ -1945,7 +2009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2878,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D72C41-A294-471A-A10F-81DBDBC72609}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3074,6 +3140,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BBCB75-CC54-4A68-8714-84B24CB5E606}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Manas's Commit 17th Mar 04:16 p.m.
</commit_message>
<xml_diff>
--- a/testData/TestData_CPQ_Automation.xlsx
+++ b/testData/TestData_CPQ_Automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnayak\PycharmProjects\OneStopCPQ\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF3A8A2-6D9A-4D4D-BA58-2BA1ABF633D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBA608-220D-4661-971D-981298655573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs Status" sheetId="18" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="TC_016" sheetId="17" r:id="rId18"/>
     <sheet name="TC_017" sheetId="19" r:id="rId19"/>
     <sheet name="TC_018" sheetId="20" r:id="rId20"/>
+    <sheet name="TC_019" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="302">
   <si>
     <t>Test Name</t>
   </si>
@@ -907,6 +908,54 @@
   </si>
   <si>
     <t>test_CR_Exclusion_Disable_Selection_TP</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Prompt_Selection_Classic</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Prompt_Selection_Split</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Prompt_Selection_TP</t>
+  </si>
+  <si>
+    <t>test_CR_Exclusion_Prompt_Selection_TC</t>
+  </si>
+  <si>
+    <t>Same prompt is shown for 2nd CR too</t>
+  </si>
+  <si>
+    <t>test_TC_018_AllowManualAdj_False</t>
+  </si>
+  <si>
+    <t>test_AllowManualAdj_False_Classic</t>
+  </si>
+  <si>
+    <t>test_AllowManualAdj_False_Split</t>
+  </si>
+  <si>
+    <t>test_AllowManualAdj_False_TP</t>
+  </si>
+  <si>
+    <t>test_AllowManualAdj_False_TC</t>
+  </si>
+  <si>
+    <t>Data sync not happening for TC</t>
+  </si>
+  <si>
+    <t>test_DirectConfiguration</t>
+  </si>
+  <si>
+    <t>MN - 2020 Proposal TC_019</t>
+  </si>
+  <si>
+    <t>MN - 2020 PL(GBP)</t>
+  </si>
+  <si>
+    <t>MN - 2020 Option A(GBP)</t>
+  </si>
+  <si>
+    <t>MN - 2020 BUNDLE (GBP)</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE8C29B-2DBF-44E9-93DE-0354258C5C49}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1839,12 +1888,88 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49" s="9" t="s">
         <v>285</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>18</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2944,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D72C41-A294-471A-A10F-81DBDBC72609}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,7 +3272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BBCB75-CC54-4A68-8714-84B24CB5E606}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3227,6 +3354,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C25FC0-E9CE-48B4-B18D-4B2DFAE7BC8E}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>